<commit_message>
updated debug the FDA_EUA_v3x OWL and ontorat files.
</commit_message>
<xml_diff>
--- a/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
+++ b/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linay\ontologies\GitHub\cido\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linay\ontologies\GitHub\cido\docs\FDA_EUA tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD92F54-698E-4B51-8569-6BBA2D239DF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA896E3-8088-48D1-AF0A-602A2B2C18C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2CB072C4-4071-45ED-9E21-A7B6C58CD755}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5837" uniqueCount="2570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5837" uniqueCount="2566">
   <si>
     <t>Company/Organization</t>
   </si>
@@ -7709,15 +7709,6 @@
     <t xml:space="preserve">http://purl.obolibrary.org/obo/OGG_3043740570 </t>
   </si>
   <si>
-    <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_30437405781a</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OGG_30437405781a</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OGG_30437405781</t>
-  </si>
-  <si>
     <t>orf1ab,RdRp,ORF1a,ORF1</t>
   </si>
   <si>
@@ -7800,9 +7791,6 @@
   </si>
   <si>
     <t>genome of severe acute respiratory syndrome coronavirus 2'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_30437405781</t>
   </si>
 </sst>
 </file>
@@ -8204,8 +8192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6338C626-B5C7-4274-B4C3-F95CCA523B46}">
   <dimension ref="A1:V346"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:V344"/>
+    <sheetView tabSelected="1" topLeftCell="F312" workbookViewId="0">
+      <selection activeCell="N327" sqref="A1:V344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8282,7 +8270,7 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="U1" t="s">
         <v>14</v>
@@ -8999,7 +8987,7 @@
         <v>442</v>
       </c>
       <c r="B16" t="s">
-        <v>2551</v>
+        <v>2548</v>
       </c>
       <c r="C16" t="s">
         <v>443</v>
@@ -10419,7 +10407,7 @@
         <v>989</v>
       </c>
       <c r="M42" t="s">
-        <v>2540</v>
+        <v>2528</v>
       </c>
       <c r="N42" t="s">
         <v>2536</v>
@@ -10475,7 +10463,7 @@
         <v>649</v>
       </c>
       <c r="M43" t="s">
-        <v>2539</v>
+        <v>2528</v>
       </c>
       <c r="S43" t="s">
         <v>378</v>
@@ -10781,7 +10769,7 @@
         <v>423</v>
       </c>
       <c r="U49" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V49" t="s">
         <v>30</v>
@@ -11237,7 +11225,7 @@
         <v>2527</v>
       </c>
       <c r="N58" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="S58" t="s">
         <v>490</v>
@@ -12341,7 +12329,7 @@
         <v>65</v>
       </c>
       <c r="J79" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K79" t="s">
         <v>308</v>
@@ -12350,7 +12338,7 @@
         <v>309</v>
       </c>
       <c r="M79" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="S79" t="s">
         <v>628</v>
@@ -12506,7 +12494,7 @@
         <v>12</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
       <c r="K82" t="s">
         <v>527</v>
@@ -12724,7 +12712,7 @@
         <v>679</v>
       </c>
       <c r="U86" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V86" t="s">
         <v>30</v>
@@ -12771,7 +12759,7 @@
         <v>688</v>
       </c>
       <c r="U87" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V87" t="s">
         <v>30</v>
@@ -12877,7 +12865,7 @@
         <v>2535</v>
       </c>
       <c r="P89" t="s">
-        <v>2538</v>
+        <v>2533</v>
       </c>
       <c r="S89" t="s">
         <v>702</v>
@@ -13433,7 +13421,7 @@
         <v>491</v>
       </c>
       <c r="B100" t="s">
-        <v>2558</v>
+        <v>2555</v>
       </c>
       <c r="C100" t="s">
         <v>492</v>
@@ -13486,7 +13474,7 @@
         <v>166</v>
       </c>
       <c r="B101" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="C101" t="s">
         <v>2341</v>
@@ -14287,7 +14275,7 @@
         <v>469</v>
       </c>
       <c r="B116" t="s">
-        <v>2555</v>
+        <v>2552</v>
       </c>
       <c r="C116" t="s">
         <v>470</v>
@@ -15097,7 +15085,7 @@
         <v>998</v>
       </c>
       <c r="U131" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V131" t="s">
         <v>30</v>
@@ -15356,7 +15344,7 @@
         <v>1031</v>
       </c>
       <c r="U136" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V136" t="s">
         <v>30</v>
@@ -15400,7 +15388,7 @@
         <v>1037</v>
       </c>
       <c r="U137" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V137" t="s">
         <v>30</v>
@@ -15411,7 +15399,7 @@
         <v>462</v>
       </c>
       <c r="B138" t="s">
-        <v>2554</v>
+        <v>2551</v>
       </c>
       <c r="C138" t="s">
         <v>463</v>
@@ -16366,7 +16354,7 @@
         <v>1159</v>
       </c>
       <c r="U155" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V155" t="s">
         <v>30</v>
@@ -16457,7 +16445,7 @@
         <v>1172</v>
       </c>
       <c r="U157" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V157" t="s">
         <v>30</v>
@@ -16816,7 +16804,7 @@
         <v>65</v>
       </c>
       <c r="J164" s="3" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K164" t="s">
         <v>1087</v>
@@ -17034,7 +17022,7 @@
         <v>65</v>
       </c>
       <c r="J168" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K168" t="s">
         <v>359</v>
@@ -17367,7 +17355,7 @@
         <v>65</v>
       </c>
       <c r="J174" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K174" t="s">
         <v>1634</v>
@@ -17376,7 +17364,7 @@
         <v>474</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="S174" t="s">
         <v>1285</v>
@@ -17552,7 +17540,7 @@
         <v>456</v>
       </c>
       <c r="B178" t="s">
-        <v>2553</v>
+        <v>2550</v>
       </c>
       <c r="C178" t="s">
         <v>457</v>
@@ -17856,7 +17844,7 @@
         <v>1347</v>
       </c>
       <c r="U183" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V183" t="s">
         <v>30</v>
@@ -18424,7 +18412,7 @@
         <v>649</v>
       </c>
       <c r="M194" t="s">
-        <v>2539</v>
+        <v>2528</v>
       </c>
       <c r="S194" t="s">
         <v>1426</v>
@@ -18915,7 +18903,7 @@
         <v>2366</v>
       </c>
       <c r="B204" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="C204" t="s">
         <v>2368</v>
@@ -19230,7 +19218,7 @@
         <v>449</v>
       </c>
       <c r="B210" t="s">
-        <v>2552</v>
+        <v>2549</v>
       </c>
       <c r="C210" t="s">
         <v>450</v>
@@ -19743,7 +19731,7 @@
         <v>2528</v>
       </c>
       <c r="N219" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="S219" t="s">
         <v>1606</v>
@@ -19905,7 +19893,7 @@
         <v>1629</v>
       </c>
       <c r="U222" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V222" t="s">
         <v>30</v>
@@ -20055,7 +20043,7 @@
         <v>1647</v>
       </c>
       <c r="U225" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V225" t="s">
         <v>30</v>
@@ -20753,7 +20741,7 @@
         <v>1740</v>
       </c>
       <c r="U238" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V238" t="s">
         <v>30</v>
@@ -21618,7 +21606,7 @@
         <v>1865</v>
       </c>
       <c r="U255" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V255" t="s">
         <v>30</v>
@@ -21968,7 +21956,7 @@
         <v>1916</v>
       </c>
       <c r="U262" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V262" t="s">
         <v>30</v>
@@ -22748,7 +22736,7 @@
         <v>65</v>
       </c>
       <c r="J277" s="3" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K277" t="s">
         <v>518</v>
@@ -22757,7 +22745,7 @@
         <v>519</v>
       </c>
       <c r="M277" s="3" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="S277" t="s">
         <v>2021</v>
@@ -23039,7 +23027,7 @@
         <v>476</v>
       </c>
       <c r="B283" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
       <c r="C283" t="s">
         <v>477</v>
@@ -23443,7 +23431,7 @@
         <v>440</v>
       </c>
       <c r="U290" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="V290" t="s">
         <v>441</v>
@@ -24676,7 +24664,7 @@
         <v>65</v>
       </c>
       <c r="J314" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="K314" t="s">
         <v>249</v>
@@ -25380,7 +25368,7 @@
         <v>2524</v>
       </c>
       <c r="N327" t="s">
-        <v>2569</v>
+        <v>2533</v>
       </c>
       <c r="S327" t="s">
         <v>2379</v>
@@ -26239,13 +26227,13 @@
         <v>510</v>
       </c>
       <c r="B344" t="s">
-        <v>2562</v>
+        <v>2559</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>511</v>
       </c>
       <c r="D344" s="3" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="E344" s="4" t="s">
         <v>149</v>
@@ -26266,10 +26254,10 @@
         <v>440</v>
       </c>
       <c r="K344" s="3" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="L344" s="3" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
       <c r="M344" s="3" t="s">
         <v>2524</v>
@@ -26352,7 +26340,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2528</v>
@@ -26384,7 +26372,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2542</v>
+        <v>2539</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2524</v>
@@ -26395,10 +26383,10 @@
         <v>519</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2568</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -26472,10 +26460,10 @@
         <v>248</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -26486,18 +26474,18 @@
         <v>1881</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2546</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>2548</v>
+        <v>2545</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1897</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2547</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -26513,7 +26501,7 @@
         <v>1861</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2550</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -26526,10 +26514,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="C19" t="s">
-        <v>2561</v>
+        <v>2558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the ORF1ab OGGID error, and updated the cido-base and cido file
</commit_message>
<xml_diff>
--- a/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
+++ b/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linay\ontologies\GitHub\cido\docs\FDA_EUA tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA896E3-8088-48D1-AF0A-602A2B2C18C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A36935-0466-48AB-BDA6-E2B9FD53C8A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2CB072C4-4071-45ED-9E21-A7B6C58CD755}"/>
   </bookViews>
@@ -7679,9 +7679,6 @@
     <t>http://purl.obolibrary.org/obo/OGG_3043740568</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/OGG_3043740578</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CIDO_0000351</t>
   </si>
   <si>
@@ -7694,12 +7691,6 @@
     <t xml:space="preserve">http://purl.obolibrary.org/obo/OGG_3043740575 </t>
   </si>
   <si>
-    <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_3043740578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://purl.obolibrary.org/obo/OGG_3043740578 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_3043740568</t>
   </si>
   <si>
@@ -7791,6 +7782,15 @@
   </si>
   <si>
     <t>genome of severe acute respiratory syndrome coronavirus 2'</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OGG_3043740579</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_3043740579</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OGG_3043740579 </t>
   </si>
 </sst>
 </file>
@@ -8192,8 +8192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6338C626-B5C7-4274-B4C3-F95CCA523B46}">
   <dimension ref="A1:V346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F312" workbookViewId="0">
-      <selection activeCell="N327" sqref="A1:V344"/>
+    <sheetView tabSelected="1" topLeftCell="O317" workbookViewId="0">
+      <selection sqref="A1:V344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8270,7 +8270,7 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
-        <v>2540</v>
+        <v>2537</v>
       </c>
       <c r="U1" t="s">
         <v>14</v>
@@ -8317,7 +8317,7 @@
         <v>1895</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N2" t="s">
         <v>2526</v>
@@ -8373,7 +8373,7 @@
         <v>1887</v>
       </c>
       <c r="M3" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S3" t="s">
         <v>38</v>
@@ -8449,7 +8449,7 @@
         <v>54</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K5" t="s">
         <v>45</v>
@@ -8499,7 +8499,7 @@
         <v>92</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K6" t="s">
         <v>93</v>
@@ -8602,7 +8602,7 @@
         <v>141</v>
       </c>
       <c r="J8" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K8" t="s">
         <v>142</v>
@@ -8658,13 +8658,13 @@
         <v>1479</v>
       </c>
       <c r="M9" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N9" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O9" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S9" t="s">
         <v>95</v>
@@ -8755,7 +8755,7 @@
         <v>44</v>
       </c>
       <c r="J11" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K11" t="s">
         <v>45</v>
@@ -8902,7 +8902,7 @@
         <v>92</v>
       </c>
       <c r="J14" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K14" t="s">
         <v>93</v>
@@ -8964,10 +8964,10 @@
         <v>2524</v>
       </c>
       <c r="N15" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="O15" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S15" t="s">
         <v>143</v>
@@ -8987,7 +8987,7 @@
         <v>442</v>
       </c>
       <c r="B16" t="s">
-        <v>2548</v>
+        <v>2545</v>
       </c>
       <c r="C16" t="s">
         <v>443</v>
@@ -9020,7 +9020,7 @@
         <v>447</v>
       </c>
       <c r="M16" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S16" t="s">
         <v>154</v>
@@ -9076,7 +9076,7 @@
         <v>2526</v>
       </c>
       <c r="N17" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S17" t="s">
         <v>164</v>
@@ -9132,7 +9132,7 @@
         <v>2524</v>
       </c>
       <c r="N18" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S18" t="s">
         <v>172</v>
@@ -9185,10 +9185,10 @@
         <v>563</v>
       </c>
       <c r="M19" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N19" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S19" t="s">
         <v>179</v>
@@ -9241,7 +9241,7 @@
         <v>1887</v>
       </c>
       <c r="M20" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S20" t="s">
         <v>188</v>
@@ -9294,7 +9294,7 @@
         <v>1793</v>
       </c>
       <c r="M21" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S21" t="s">
         <v>196</v>
@@ -9347,7 +9347,7 @@
         <v>447</v>
       </c>
       <c r="M22" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S22" t="s">
         <v>203</v>
@@ -9400,7 +9400,7 @@
         <v>2080</v>
       </c>
       <c r="M23" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N23" t="s">
         <v>2524</v>
@@ -9459,13 +9459,13 @@
         <v>586</v>
       </c>
       <c r="M24" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N24" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O24" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S24" t="s">
         <v>220</v>
@@ -9612,7 +9612,7 @@
         <v>233</v>
       </c>
       <c r="J27" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K27" t="s">
         <v>2121</v>
@@ -9671,7 +9671,7 @@
         <v>163</v>
       </c>
       <c r="M28" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S28" t="s">
         <v>250</v>
@@ -9715,7 +9715,7 @@
         <v>65</v>
       </c>
       <c r="J29" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K29" t="s">
         <v>132</v>
@@ -9724,7 +9724,7 @@
         <v>133</v>
       </c>
       <c r="M29" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S29" t="s">
         <v>260</v>
@@ -9777,7 +9777,7 @@
         <v>163</v>
       </c>
       <c r="M30" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S30" t="s">
         <v>269</v>
@@ -9830,10 +9830,10 @@
         <v>259</v>
       </c>
       <c r="M31" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N31" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S31" t="s">
         <v>276</v>
@@ -9886,7 +9886,7 @@
         <v>489</v>
       </c>
       <c r="M32" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N32" t="s">
         <v>2524</v>
@@ -10092,7 +10092,7 @@
         <v>233</v>
       </c>
       <c r="J36" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K36" t="s">
         <v>1344</v>
@@ -10407,10 +10407,10 @@
         <v>989</v>
       </c>
       <c r="M42" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N42" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S42" t="s">
         <v>370</v>
@@ -10463,7 +10463,7 @@
         <v>649</v>
       </c>
       <c r="M43" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S43" t="s">
         <v>378</v>
@@ -10657,7 +10657,7 @@
         <v>12</v>
       </c>
       <c r="J47" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K47" t="s">
         <v>67</v>
@@ -10707,7 +10707,7 @@
         <v>12</v>
       </c>
       <c r="J48" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K48" t="s">
         <v>67</v>
@@ -10769,7 +10769,7 @@
         <v>423</v>
       </c>
       <c r="U49" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V49" t="s">
         <v>30</v>
@@ -10804,7 +10804,7 @@
         <v>233</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K50" t="s">
         <v>392</v>
@@ -10851,7 +10851,7 @@
         <v>54</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K51" t="s">
         <v>844</v>
@@ -10901,7 +10901,7 @@
         <v>92</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K52" t="s">
         <v>844</v>
@@ -11066,7 +11066,7 @@
         <v>1778</v>
       </c>
       <c r="M55" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S55" t="s">
         <v>468</v>
@@ -11119,7 +11119,7 @@
         <v>2210</v>
       </c>
       <c r="M56" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S56" s="3" t="s">
         <v>475</v>
@@ -11225,7 +11225,7 @@
         <v>2527</v>
       </c>
       <c r="N58" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="S58" t="s">
         <v>490</v>
@@ -11322,7 +11322,7 @@
         <v>233</v>
       </c>
       <c r="J60" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K60" t="s">
         <v>1575</v>
@@ -11381,10 +11381,10 @@
         <v>1129</v>
       </c>
       <c r="M61" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N61" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S61" t="s">
         <v>509</v>
@@ -11590,7 +11590,7 @@
         <v>163</v>
       </c>
       <c r="M65" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S65" t="s">
         <v>528</v>
@@ -11634,7 +11634,7 @@
         <v>233</v>
       </c>
       <c r="J66" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K66" t="s">
         <v>142</v>
@@ -11749,10 +11749,10 @@
         <v>2524</v>
       </c>
       <c r="N68" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="O68" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S68" t="s">
         <v>549</v>
@@ -11796,7 +11796,7 @@
         <v>12</v>
       </c>
       <c r="J69" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K69" t="s">
         <v>37</v>
@@ -11846,7 +11846,7 @@
         <v>233</v>
       </c>
       <c r="J70" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K70" t="s">
         <v>142</v>
@@ -11908,7 +11908,7 @@
         <v>2524</v>
       </c>
       <c r="N71" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S71" t="s">
         <v>572</v>
@@ -12070,7 +12070,7 @@
         <v>2526</v>
       </c>
       <c r="N74" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S74" t="s">
         <v>594</v>
@@ -12176,7 +12176,7 @@
         <v>2142</v>
       </c>
       <c r="M76" t="s">
-        <v>2537</v>
+        <v>2534</v>
       </c>
       <c r="N76" s="3" t="s">
         <v>2527</v>
@@ -12232,7 +12232,7 @@
         <v>467</v>
       </c>
       <c r="M77" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S77" t="s">
         <v>614</v>
@@ -12285,7 +12285,7 @@
         <v>163</v>
       </c>
       <c r="M78" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S78" t="s">
         <v>621</v>
@@ -12329,7 +12329,7 @@
         <v>65</v>
       </c>
       <c r="J79" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K79" t="s">
         <v>308</v>
@@ -12338,7 +12338,7 @@
         <v>309</v>
       </c>
       <c r="M79" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="S79" t="s">
         <v>628</v>
@@ -12394,7 +12394,7 @@
         <v>2526</v>
       </c>
       <c r="N80" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S80" t="s">
         <v>635</v>
@@ -12450,10 +12450,10 @@
         <v>2524</v>
       </c>
       <c r="N81" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="O81" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S81" t="s">
         <v>643</v>
@@ -12494,7 +12494,7 @@
         <v>12</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>2546</v>
+        <v>2543</v>
       </c>
       <c r="K82" t="s">
         <v>527</v>
@@ -12553,7 +12553,7 @@
         <v>2461</v>
       </c>
       <c r="M83" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S83" t="s">
         <v>657</v>
@@ -12606,10 +12606,10 @@
         <v>1035</v>
       </c>
       <c r="M84" t="s">
+        <v>2564</v>
+      </c>
+      <c r="N84" t="s">
         <v>2533</v>
-      </c>
-      <c r="N84" t="s">
-        <v>2536</v>
       </c>
       <c r="S84" t="s">
         <v>664</v>
@@ -12662,10 +12662,10 @@
         <v>343</v>
       </c>
       <c r="M85" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N85" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S85" t="s">
         <v>672</v>
@@ -12712,7 +12712,7 @@
         <v>679</v>
       </c>
       <c r="U86" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V86" t="s">
         <v>30</v>
@@ -12759,7 +12759,7 @@
         <v>688</v>
       </c>
       <c r="U87" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V87" t="s">
         <v>30</v>
@@ -12803,7 +12803,7 @@
         <v>1793</v>
       </c>
       <c r="M88" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S88" t="s">
         <v>694</v>
@@ -12859,13 +12859,13 @@
         <v>2524</v>
       </c>
       <c r="N89" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="O89" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="P89" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S89" t="s">
         <v>702</v>
@@ -12918,7 +12918,7 @@
         <v>163</v>
       </c>
       <c r="M90" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S90" t="s">
         <v>709</v>
@@ -12971,13 +12971,13 @@
         <v>1479</v>
       </c>
       <c r="M91" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N91" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O91" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S91" t="s">
         <v>716</v>
@@ -13083,10 +13083,10 @@
         <v>1568</v>
       </c>
       <c r="M93" t="s">
-        <v>2534</v>
+        <v>2565</v>
       </c>
       <c r="N93" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S93" t="s">
         <v>727</v>
@@ -13230,7 +13230,7 @@
         <v>1858</v>
       </c>
       <c r="J96" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K96" t="s">
         <v>1878</v>
@@ -13289,7 +13289,7 @@
         <v>438</v>
       </c>
       <c r="M97" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="S97" t="s">
         <v>756</v>
@@ -13342,10 +13342,10 @@
         <v>259</v>
       </c>
       <c r="M98" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N98" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S98" t="s">
         <v>764</v>
@@ -13398,10 +13398,10 @@
         <v>1451</v>
       </c>
       <c r="M99" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N99" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S99" t="s">
         <v>771</v>
@@ -13421,7 +13421,7 @@
         <v>491</v>
       </c>
       <c r="B100" t="s">
-        <v>2555</v>
+        <v>2552</v>
       </c>
       <c r="C100" t="s">
         <v>492</v>
@@ -13474,7 +13474,7 @@
         <v>166</v>
       </c>
       <c r="B101" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
       <c r="C101" t="s">
         <v>2341</v>
@@ -13610,13 +13610,13 @@
         <v>586</v>
       </c>
       <c r="M103" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N103" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O103" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S103" t="s">
         <v>801</v>
@@ -13719,7 +13719,7 @@
         <v>1232</v>
       </c>
       <c r="M105" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S105" t="s">
         <v>816</v>
@@ -14093,10 +14093,10 @@
         <v>2524</v>
       </c>
       <c r="N112" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="O112" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S112" t="s">
         <v>866</v>
@@ -14149,10 +14149,10 @@
         <v>1029</v>
       </c>
       <c r="M113" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N113" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S113" t="s">
         <v>874</v>
@@ -14205,7 +14205,7 @@
         <v>1871</v>
       </c>
       <c r="M114" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S114" t="s">
         <v>882</v>
@@ -14249,7 +14249,7 @@
         <v>92</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K115" t="s">
         <v>45</v>
@@ -14275,7 +14275,7 @@
         <v>469</v>
       </c>
       <c r="B116" t="s">
-        <v>2552</v>
+        <v>2549</v>
       </c>
       <c r="C116" t="s">
         <v>470</v>
@@ -14399,7 +14399,7 @@
         <v>92</v>
       </c>
       <c r="J118" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K118" t="s">
         <v>399</v>
@@ -14446,7 +14446,7 @@
         <v>54</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K119" t="s">
         <v>45</v>
@@ -14546,7 +14546,7 @@
         <v>54</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K121" t="s">
         <v>45</v>
@@ -14658,7 +14658,7 @@
         <v>2524</v>
       </c>
       <c r="N123" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S123" t="s">
         <v>941</v>
@@ -14767,10 +14767,10 @@
         <v>2524</v>
       </c>
       <c r="N125" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="O125" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S125" t="s">
         <v>951</v>
@@ -14826,10 +14826,10 @@
         <v>2524</v>
       </c>
       <c r="N126" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="O126" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S126" t="s">
         <v>958</v>
@@ -14923,7 +14923,7 @@
         <v>195</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K128" t="s">
         <v>45</v>
@@ -15023,7 +15023,7 @@
         <v>12</v>
       </c>
       <c r="J130" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K130" t="s">
         <v>25</v>
@@ -15085,7 +15085,7 @@
         <v>998</v>
       </c>
       <c r="U131" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V131" t="s">
         <v>30</v>
@@ -15232,7 +15232,7 @@
         <v>2524</v>
       </c>
       <c r="N134" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S134" t="s">
         <v>1016</v>
@@ -15285,10 +15285,10 @@
         <v>259</v>
       </c>
       <c r="M135" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N135" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S135" t="s">
         <v>1022</v>
@@ -15344,7 +15344,7 @@
         <v>1031</v>
       </c>
       <c r="U136" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V136" t="s">
         <v>30</v>
@@ -15388,7 +15388,7 @@
         <v>1037</v>
       </c>
       <c r="U137" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V137" t="s">
         <v>30</v>
@@ -15399,7 +15399,7 @@
         <v>462</v>
       </c>
       <c r="B138" t="s">
-        <v>2551</v>
+        <v>2548</v>
       </c>
       <c r="C138" t="s">
         <v>463</v>
@@ -15432,7 +15432,7 @@
         <v>467</v>
       </c>
       <c r="M138" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S138" t="s">
         <v>1041</v>
@@ -15538,7 +15538,7 @@
         <v>447</v>
       </c>
       <c r="M140" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S140" t="s">
         <v>1055</v>
@@ -15591,13 +15591,13 @@
         <v>1656</v>
       </c>
       <c r="M141" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N141" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O141" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S141" t="s">
         <v>1062</v>
@@ -15650,10 +15650,10 @@
         <v>686</v>
       </c>
       <c r="M142" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N142" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S142" t="s">
         <v>1068</v>
@@ -15706,10 +15706,10 @@
         <v>1500</v>
       </c>
       <c r="M143" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N143" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S143" t="s">
         <v>1077</v>
@@ -15762,7 +15762,7 @@
         <v>1793</v>
       </c>
       <c r="M144" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S144" t="s">
         <v>1081</v>
@@ -15806,7 +15806,7 @@
         <v>233</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K145" t="s">
         <v>268</v>
@@ -15918,7 +15918,7 @@
         <v>1871</v>
       </c>
       <c r="M147" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S147" t="s">
         <v>1102</v>
@@ -16077,7 +16077,7 @@
         <v>1793</v>
       </c>
       <c r="M150" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S150" t="s">
         <v>1122</v>
@@ -16130,10 +16130,10 @@
         <v>1525</v>
       </c>
       <c r="M151" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N151" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S151" t="s">
         <v>1130</v>
@@ -16289,10 +16289,10 @@
         <v>259</v>
       </c>
       <c r="M154" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N154" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S154" t="s">
         <v>1150</v>
@@ -16345,7 +16345,7 @@
         <v>163</v>
       </c>
       <c r="M155" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S155" t="s">
         <v>1158</v>
@@ -16354,7 +16354,7 @@
         <v>1159</v>
       </c>
       <c r="U155" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V155" t="s">
         <v>30</v>
@@ -16445,7 +16445,7 @@
         <v>1172</v>
       </c>
       <c r="U157" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V157" t="s">
         <v>30</v>
@@ -16701,13 +16701,13 @@
         <v>586</v>
       </c>
       <c r="M162" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N162" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O162" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S162" t="s">
         <v>1206</v>
@@ -16760,7 +16760,7 @@
         <v>1793</v>
       </c>
       <c r="M163" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S163" t="s">
         <v>1210</v>
@@ -16804,7 +16804,7 @@
         <v>65</v>
       </c>
       <c r="J164" s="3" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K164" t="s">
         <v>1087</v>
@@ -16972,13 +16972,13 @@
         <v>1479</v>
       </c>
       <c r="M167" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N167" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O167" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S167" t="s">
         <v>1241</v>
@@ -17022,7 +17022,7 @@
         <v>65</v>
       </c>
       <c r="J168" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K168" t="s">
         <v>359</v>
@@ -17087,10 +17087,10 @@
         <v>2524</v>
       </c>
       <c r="N169" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="O169" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S169" t="s">
         <v>1254</v>
@@ -17196,10 +17196,10 @@
         <v>489</v>
       </c>
       <c r="M171" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N171" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S171" t="s">
         <v>1266</v>
@@ -17252,13 +17252,13 @@
         <v>873</v>
       </c>
       <c r="M172" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N172" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O172" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S172" t="s">
         <v>1271</v>
@@ -17311,7 +17311,7 @@
         <v>2157</v>
       </c>
       <c r="M173" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S173" t="s">
         <v>1279</v>
@@ -17355,7 +17355,7 @@
         <v>65</v>
       </c>
       <c r="J174" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K174" t="s">
         <v>1634</v>
@@ -17364,7 +17364,7 @@
         <v>474</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="S174" t="s">
         <v>1285</v>
@@ -17514,7 +17514,7 @@
         <v>141</v>
       </c>
       <c r="J177" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K177" t="s">
         <v>142</v>
@@ -17540,7 +17540,7 @@
         <v>456</v>
       </c>
       <c r="B178" t="s">
-        <v>2550</v>
+        <v>2547</v>
       </c>
       <c r="C178" t="s">
         <v>457</v>
@@ -17626,13 +17626,13 @@
         <v>1493</v>
       </c>
       <c r="M179" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N179" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="O179" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S179" t="s">
         <v>1315</v>
@@ -17685,10 +17685,10 @@
         <v>1029</v>
       </c>
       <c r="M180" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N180" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S180" t="s">
         <v>1322</v>
@@ -17741,7 +17741,7 @@
         <v>163</v>
       </c>
       <c r="M181" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S181" t="s">
         <v>1329</v>
@@ -17844,7 +17844,7 @@
         <v>1347</v>
       </c>
       <c r="U183" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V183" t="s">
         <v>30</v>
@@ -17888,7 +17888,7 @@
         <v>1895</v>
       </c>
       <c r="M184" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N184" t="s">
         <v>2526</v>
@@ -17947,7 +17947,7 @@
         <v>2524</v>
       </c>
       <c r="N185" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S185" t="s">
         <v>1358</v>
@@ -18412,7 +18412,7 @@
         <v>649</v>
       </c>
       <c r="M194" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S194" t="s">
         <v>1426</v>
@@ -18465,7 +18465,7 @@
         <v>163</v>
       </c>
       <c r="M195" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S195" t="s">
         <v>1431</v>
@@ -18509,7 +18509,7 @@
         <v>233</v>
       </c>
       <c r="J196" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K196" t="s">
         <v>1386</v>
@@ -18568,7 +18568,7 @@
         <v>163</v>
       </c>
       <c r="M197" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S197" t="s">
         <v>1444</v>
@@ -18621,7 +18621,7 @@
         <v>163</v>
       </c>
       <c r="M198" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S198" t="s">
         <v>1452</v>
@@ -18665,7 +18665,7 @@
         <v>233</v>
       </c>
       <c r="J199" s="3" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K199" t="s">
         <v>844</v>
@@ -18727,7 +18727,7 @@
         <v>2524</v>
       </c>
       <c r="N200" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S200" t="s">
         <v>1465</v>
@@ -18780,7 +18780,7 @@
         <v>125</v>
       </c>
       <c r="M201" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S201" t="s">
         <v>1472</v>
@@ -18903,7 +18903,7 @@
         <v>2366</v>
       </c>
       <c r="B204" t="s">
-        <v>2554</v>
+        <v>2551</v>
       </c>
       <c r="C204" t="s">
         <v>2368</v>
@@ -19033,7 +19033,7 @@
         <v>141</v>
       </c>
       <c r="J206" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K206" t="s">
         <v>734</v>
@@ -19148,7 +19148,7 @@
         <v>2524</v>
       </c>
       <c r="N208" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S208" t="s">
         <v>1526</v>
@@ -19218,7 +19218,7 @@
         <v>449</v>
       </c>
       <c r="B210" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
       <c r="C210" t="s">
         <v>450</v>
@@ -19357,7 +19357,7 @@
         <v>1887</v>
       </c>
       <c r="M212" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S212" t="s">
         <v>1552</v>
@@ -19410,7 +19410,7 @@
         <v>2394</v>
       </c>
       <c r="M213" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S213" t="s">
         <v>1561</v>
@@ -19557,7 +19557,7 @@
         <v>233</v>
       </c>
       <c r="J216" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K216" t="s">
         <v>45</v>
@@ -19616,7 +19616,7 @@
         <v>489</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N217" t="s">
         <v>2524</v>
@@ -19675,7 +19675,7 @@
         <v>2524</v>
       </c>
       <c r="N218" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S218" t="s">
         <v>1599</v>
@@ -19728,10 +19728,10 @@
         <v>571</v>
       </c>
       <c r="M219" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N219" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="S219" t="s">
         <v>1606</v>
@@ -19784,7 +19784,7 @@
         <v>1793</v>
       </c>
       <c r="M220" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S220" t="s">
         <v>1613</v>
@@ -19893,7 +19893,7 @@
         <v>1629</v>
       </c>
       <c r="U222" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V222" t="s">
         <v>30</v>
@@ -20043,7 +20043,7 @@
         <v>1647</v>
       </c>
       <c r="U225" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V225" t="s">
         <v>30</v>
@@ -20087,7 +20087,7 @@
         <v>1232</v>
       </c>
       <c r="M226" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S226" t="s">
         <v>1650</v>
@@ -20131,7 +20131,7 @@
         <v>233</v>
       </c>
       <c r="J227" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K227" t="s">
         <v>45</v>
@@ -20296,7 +20296,7 @@
         <v>1837</v>
       </c>
       <c r="M230" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S230" t="s">
         <v>1678</v>
@@ -20402,7 +20402,7 @@
         <v>2309</v>
       </c>
       <c r="M232" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S232" t="s">
         <v>1693</v>
@@ -20458,10 +20458,10 @@
         <v>2524</v>
       </c>
       <c r="N233" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="O233" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="Q233" t="s">
         <v>474</v>
@@ -20517,10 +20517,10 @@
         <v>489</v>
       </c>
       <c r="M234" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N234" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S234" t="s">
         <v>1708</v>
@@ -20573,7 +20573,7 @@
         <v>1895</v>
       </c>
       <c r="M235" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N235" t="s">
         <v>2526</v>
@@ -20629,10 +20629,10 @@
         <v>259</v>
       </c>
       <c r="M236" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N236" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S236" t="s">
         <v>1723</v>
@@ -20741,7 +20741,7 @@
         <v>1740</v>
       </c>
       <c r="U238" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V238" t="s">
         <v>30</v>
@@ -20888,7 +20888,7 @@
         <v>163</v>
       </c>
       <c r="M241" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S241" t="s">
         <v>1762</v>
@@ -20941,10 +20941,10 @@
         <v>1029</v>
       </c>
       <c r="M242" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N242" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S242" t="s">
         <v>1770</v>
@@ -20997,7 +20997,7 @@
         <v>163</v>
       </c>
       <c r="M243" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S243" t="s">
         <v>1779</v>
@@ -21200,7 +21200,7 @@
         <v>2438</v>
       </c>
       <c r="M247" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S247" t="s">
         <v>1810</v>
@@ -21344,7 +21344,7 @@
         <v>233</v>
       </c>
       <c r="J250" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K250" t="s">
         <v>2218</v>
@@ -21403,7 +21403,7 @@
         <v>163</v>
       </c>
       <c r="M251" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S251" t="s">
         <v>1838</v>
@@ -21456,7 +21456,7 @@
         <v>1793</v>
       </c>
       <c r="M252" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S252" t="s">
         <v>1846</v>
@@ -21606,7 +21606,7 @@
         <v>1865</v>
       </c>
       <c r="U255" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V255" t="s">
         <v>30</v>
@@ -21794,7 +21794,7 @@
         <v>12</v>
       </c>
       <c r="J259" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K259" t="s">
         <v>84</v>
@@ -21844,7 +21844,7 @@
         <v>54</v>
       </c>
       <c r="J260" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K260" t="s">
         <v>708</v>
@@ -21894,7 +21894,7 @@
         <v>233</v>
       </c>
       <c r="J261" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K261" t="s">
         <v>45</v>
@@ -21956,7 +21956,7 @@
         <v>1916</v>
       </c>
       <c r="U262" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V262" t="s">
         <v>30</v>
@@ -22000,10 +22000,10 @@
         <v>1029</v>
       </c>
       <c r="M263" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N263" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S263" t="s">
         <v>1922</v>
@@ -22056,7 +22056,7 @@
         <v>2142</v>
       </c>
       <c r="M264" t="s">
-        <v>2537</v>
+        <v>2534</v>
       </c>
       <c r="N264" s="3" t="s">
         <v>2527</v>
@@ -22112,7 +22112,7 @@
         <v>163</v>
       </c>
       <c r="M265" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S265" t="s">
         <v>1937</v>
@@ -22209,7 +22209,7 @@
         <v>1645</v>
       </c>
       <c r="J267" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K267" t="s">
         <v>1715</v>
@@ -22268,7 +22268,7 @@
         <v>447</v>
       </c>
       <c r="M268" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S268" t="s">
         <v>1951</v>
@@ -22530,7 +22530,7 @@
         <v>1793</v>
       </c>
       <c r="M273" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S273" t="s">
         <v>1990</v>
@@ -22633,10 +22633,10 @@
         <v>283</v>
       </c>
       <c r="M275" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N275" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S275" t="s">
         <v>2006</v>
@@ -22689,7 +22689,7 @@
         <v>489</v>
       </c>
       <c r="M276" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N276" t="s">
         <v>2524</v>
@@ -22736,7 +22736,7 @@
         <v>65</v>
       </c>
       <c r="J277" s="3" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K277" t="s">
         <v>518</v>
@@ -22745,7 +22745,7 @@
         <v>519</v>
       </c>
       <c r="M277" s="3" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="S277" t="s">
         <v>2021</v>
@@ -22901,7 +22901,7 @@
         <v>1829</v>
       </c>
       <c r="M280" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S280" t="s">
         <v>2044</v>
@@ -22954,7 +22954,7 @@
         <v>1887</v>
       </c>
       <c r="M281" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S281" t="s">
         <v>2051</v>
@@ -23027,7 +23027,7 @@
         <v>476</v>
       </c>
       <c r="B283" t="s">
-        <v>2553</v>
+        <v>2550</v>
       </c>
       <c r="C283" t="s">
         <v>477</v>
@@ -23116,7 +23116,7 @@
         <v>2524</v>
       </c>
       <c r="N284" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S284" t="s">
         <v>2073</v>
@@ -23169,7 +23169,7 @@
         <v>1785</v>
       </c>
       <c r="M285" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S285" t="s">
         <v>2081</v>
@@ -23375,7 +23375,7 @@
         <v>163</v>
       </c>
       <c r="M289" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S289" t="s">
         <v>2107</v>
@@ -23431,7 +23431,7 @@
         <v>440</v>
       </c>
       <c r="U290" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="V290" t="s">
         <v>441</v>
@@ -23466,7 +23466,7 @@
         <v>54</v>
       </c>
       <c r="J291" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K291" t="s">
         <v>142</v>
@@ -23525,7 +23525,7 @@
         <v>1871</v>
       </c>
       <c r="M292" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S292" t="s">
         <v>2128</v>
@@ -23569,7 +23569,7 @@
         <v>233</v>
       </c>
       <c r="J293" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K293" t="s">
         <v>1344</v>
@@ -23728,7 +23728,7 @@
         <v>1829</v>
       </c>
       <c r="M296" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S296" t="s">
         <v>2158</v>
@@ -23781,7 +23781,7 @@
         <v>2318</v>
       </c>
       <c r="M297" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S297" t="s">
         <v>2166</v>
@@ -23878,7 +23878,7 @@
         <v>12</v>
       </c>
       <c r="J299" s="3" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K299" t="s">
         <v>837</v>
@@ -23928,7 +23928,7 @@
         <v>12</v>
       </c>
       <c r="J300" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K300" t="s">
         <v>2020</v>
@@ -24037,7 +24037,7 @@
         <v>1895</v>
       </c>
       <c r="M302" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N302" t="s">
         <v>2526</v>
@@ -24196,7 +24196,7 @@
         <v>447</v>
       </c>
       <c r="M305" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S305" t="s">
         <v>2227</v>
@@ -24252,7 +24252,7 @@
         <v>2524</v>
       </c>
       <c r="N306" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S306" t="s">
         <v>2234</v>
@@ -24296,7 +24296,7 @@
         <v>233</v>
       </c>
       <c r="J307" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K307" t="s">
         <v>45</v>
@@ -24346,7 +24346,7 @@
         <v>233</v>
       </c>
       <c r="J308" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K308" t="s">
         <v>142</v>
@@ -24408,7 +24408,7 @@
         <v>2524</v>
       </c>
       <c r="N309" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S309" t="s">
         <v>2256</v>
@@ -24461,7 +24461,7 @@
         <v>447</v>
       </c>
       <c r="M310" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S310" t="s">
         <v>2269</v>
@@ -24567,10 +24567,10 @@
         <v>1451</v>
       </c>
       <c r="M312" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N312" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S312" t="s">
         <v>2283</v>
@@ -24664,7 +24664,7 @@
         <v>65</v>
       </c>
       <c r="J314" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="K314" t="s">
         <v>249</v>
@@ -24726,10 +24726,10 @@
         <v>1224</v>
       </c>
       <c r="M315" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N315" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S315" t="s">
         <v>2304</v>
@@ -24782,7 +24782,7 @@
         <v>163</v>
       </c>
       <c r="M316" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S316" t="s">
         <v>2310</v>
@@ -24994,7 +24994,7 @@
         <v>489</v>
       </c>
       <c r="M320" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N320" t="s">
         <v>2524</v>
@@ -25050,13 +25050,13 @@
         <v>586</v>
       </c>
       <c r="M321" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N321" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="O321" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="S321" t="s">
         <v>2345</v>
@@ -25312,7 +25312,7 @@
         <v>1157</v>
       </c>
       <c r="M326" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="S326" t="s">
         <v>2371</v>
@@ -25368,7 +25368,7 @@
         <v>2524</v>
       </c>
       <c r="N327" t="s">
-        <v>2533</v>
+        <v>2564</v>
       </c>
       <c r="S327" t="s">
         <v>2379</v>
@@ -25618,7 +25618,7 @@
         <v>12</v>
       </c>
       <c r="J332" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="K332" t="s">
         <v>37</v>
@@ -25718,7 +25718,7 @@
         <v>195</v>
       </c>
       <c r="J334" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="K334" t="s">
         <v>1351</v>
@@ -25777,10 +25777,10 @@
         <v>259</v>
       </c>
       <c r="M335" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
       <c r="N335" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S335" t="s">
         <v>2439</v>
@@ -25992,7 +25992,7 @@
         <v>2526</v>
       </c>
       <c r="N339" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S339" t="s">
         <v>2469</v>
@@ -26048,7 +26048,7 @@
         <v>2526</v>
       </c>
       <c r="N340" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="S340" t="s">
         <v>2477</v>
@@ -26157,7 +26157,7 @@
         <v>2524</v>
       </c>
       <c r="N342" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="S342" t="s">
         <v>2491</v>
@@ -26227,13 +26227,13 @@
         <v>510</v>
       </c>
       <c r="B344" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>511</v>
       </c>
       <c r="D344" s="3" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="E344" s="4" t="s">
         <v>149</v>
@@ -26254,10 +26254,10 @@
         <v>440</v>
       </c>
       <c r="K344" s="3" t="s">
-        <v>2561</v>
+        <v>2558</v>
       </c>
       <c r="L344" s="3" t="s">
-        <v>2562</v>
+        <v>2559</v>
       </c>
       <c r="M344" s="3" t="s">
         <v>2524</v>
@@ -26328,7 +26328,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26340,10 +26340,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2538</v>
+        <v>2535</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2528</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -26372,7 +26372,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2539</v>
+        <v>2536</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2524</v>
@@ -26383,10 +26383,10 @@
         <v>519</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -26427,7 +26427,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="C10" t="s">
         <v>2517</v>
@@ -26438,7 +26438,7 @@
         <v>398</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2518</v>
@@ -26460,10 +26460,10 @@
         <v>248</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2542</v>
+        <v>2539</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -26474,18 +26474,18 @@
         <v>1881</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1897</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -26501,7 +26501,7 @@
         <v>1861</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>2547</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -26514,10 +26514,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="C19" t="s">
-        <v>2558</v>
+        <v>2555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ontorat FDA_EUA v3.17 updates, corrected cido-base new Chinese tests' hierarchy
</commit_message>
<xml_diff>
--- a/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
+++ b/docs/FDA_EUA tests/FDAEUA_v3_Ontorat_q.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linay\ontologies\GitHub\cido\docs\FDA_EUA tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30F9A88-FDAE-40EA-9D68-773C69FA2306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA114DB7-8518-4D77-8FE7-C284325BF241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2CB072C4-4071-45ED-9E21-A7B6C58CD755}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5891" uniqueCount="2568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5891" uniqueCount="2566">
   <si>
     <t>Company/Organization</t>
   </si>
@@ -7784,16 +7784,10 @@
     <t xml:space="preserve">http://purl.obolibrary.org/obo/OGG_3043740579 </t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/OGG_30437405791</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/OGG_3043740577</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OGG_3043740571</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> http://purl.obolibrary.org/obo/OGG_30437405791</t>
   </si>
   <si>
     <t>ORF8</t>
@@ -7880,7 +7874,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -7888,6 +7882,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10568,8 +10563,8 @@
       <c r="L42" s="6" t="s">
         <v>989</v>
       </c>
-      <c r="M42" s="6" t="s">
-        <v>2563</v>
+      <c r="M42" s="7" t="s">
+        <v>2560</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>2532</v>
@@ -10627,7 +10622,7 @@
         <v>649</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
@@ -11339,7 +11334,7 @@
         <v>2560</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
@@ -11397,7 +11392,7 @@
         <v>2526</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
@@ -11455,7 +11450,7 @@
         <v>2526</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
@@ -20516,7 +20511,7 @@
         <v>2560</v>
       </c>
       <c r="N219" s="6" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="O219" s="6"/>
       <c r="P219" s="6"/>
@@ -26629,7 +26624,7 @@
         <v>2523</v>
       </c>
       <c r="N328" s="6" t="s">
-        <v>2566</v>
+        <v>2561</v>
       </c>
       <c r="O328" s="6"/>
       <c r="P328" s="6"/>
@@ -27585,8 +27580,11 @@
     <sortCondition ref="B43:B344"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M42" r:id="rId1" display="http://purl.obolibrary.org/obo/OGG_30437405791" xr:uid="{91928038-6FAA-40D8-98FE-EB27C0AD1681}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27595,7 +27593,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27615,10 +27613,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>